<commit_message>
Updated graphs for m3
</commit_message>
<xml_diff>
--- a/Analysis/Method3/method3.xlsx
+++ b/Analysis/Method3/method3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\COP290 Design Practices\cop290_asgn1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\COP290 Design Practices\cop290_asgn1\Analysis\Method3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333708DC-FF52-4494-9150-3125A2AF4FDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A9D206-105F-4DAD-A371-5AC1BA401345}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FA81FE16-3A3A-4A97-A5F0-3D5ACD406E93}"/>
   </bookViews>
@@ -124,8 +124,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Error vs Runtime</a:t>
+              <a:t>Runtime vs</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Number of threads</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -169,11 +174,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Error</c:v>
+                  <c:v>Runtime</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -192,48 +197,66 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$6</c:f>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>256</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>259</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>315</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>365</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>481</c:v>
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$6</c:f>
+              <c:f>Sheet1!$B$2:$B$9</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.7575800000000005E-8</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>5.13E-4</c:v>
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.9543999999999998E-8</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>8.3600000000000005E-4</c:v>
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>97</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -241,7 +264,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E32D-48A3-9C5A-D45748263AB6}"/>
+              <c16:uniqueId val="{00000000-4E3A-421E-A34A-37648314A79D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -253,11 +276,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="543467728"/>
-        <c:axId val="543466128"/>
+        <c:axId val="609716408"/>
+        <c:axId val="609714808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="543467728"/>
+        <c:axId val="609716408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -314,12 +337,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="543466128"/>
+        <c:crossAx val="609714808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="543466128"/>
+        <c:axId val="609714808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -376,7 +399,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="543467728"/>
+        <c:crossAx val="609716408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -467,7 +490,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Error vs Number of threads</a:t>
+              <a:t>Error vs Runtime</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -535,48 +558,66 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:f>Sheet1!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>97</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$6</c:f>
+              <c:f>Sheet1!$C$2:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.7575800000000005E-8</c:v>
+                  <c:v>9.9677E-8</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
-                  <c:v>5.13E-4</c:v>
+                  <c:v>3.1700000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.9543999999999998E-8</c:v>
+                  <c:v>1.08871E-7</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>8.3600000000000005E-4</c:v>
+                  <c:v>5.5500000000000005E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.3100000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>5.6800000000000004E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3136400000000001E-7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -584,7 +625,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0CF2-4F56-B961-B00121953363}"/>
+              <c16:uniqueId val="{00000000-A3EC-4D76-904B-29B786AED0A2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -596,11 +637,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="543467408"/>
-        <c:axId val="543466448"/>
+        <c:axId val="609744248"/>
+        <c:axId val="609747768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="543467408"/>
+        <c:axId val="609744248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -657,12 +698,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="543466448"/>
+        <c:crossAx val="609747768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="543466448"/>
+        <c:axId val="609747768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -719,7 +760,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="543467408"/>
+        <c:crossAx val="609744248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -810,7 +851,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Runtime vs Number of threads</a:t>
+              <a:t>Error vs Number of threads</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -855,11 +896,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Sheet1!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Runtime</c:v>
+                  <c:v>Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -878,10 +919,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -896,30 +937,48 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$6</c:f>
+              <c:f>Sheet1!$C$2:$C$9</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>256</c:v>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>259</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>315</c:v>
+                  <c:v>9.9677E-8</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>3.1700000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>365</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>481</c:v>
+                  <c:v>1.08871E-7</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>5.5500000000000005E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.3100000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>5.6800000000000004E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3136400000000001E-7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -927,7 +986,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0F55-4923-BF16-A8D1FD41B2FE}"/>
+              <c16:uniqueId val="{00000000-683D-4890-BE67-677A7F5C6728}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -939,11 +998,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="506197200"/>
-        <c:axId val="506197520"/>
+        <c:axId val="609759928"/>
+        <c:axId val="609762808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="506197200"/>
+        <c:axId val="609759928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1000,12 +1059,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="506197520"/>
+        <c:crossAx val="609762808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="506197520"/>
+        <c:axId val="609762808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1062,7 +1121,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="506197200"/>
+        <c:crossAx val="609759928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2790,23 +2849,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{345697A0-86EE-4666-9EB9-7969E1CD26D9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE2BE3B7-BAD9-4925-9907-B63CB8347F72}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2826,23 +2885,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56A5EF32-A0B1-454C-98A5-5CE9D01D301E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33725304-EE22-4437-95E5-498B0E35B8EA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2862,23 +2921,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
+        <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{345311FB-161C-4A1C-88F2-6A2616453B6E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDB70CA5-EE42-4A60-97B8-27A52EE253A9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3196,10 +3255,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0141B2F1-7E95-4A3E-B455-3DEF4A384DC3}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3220,7 +3279,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>256</v>
+        <v>104</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -3231,10 +3290,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>259</v>
+        <v>94</v>
       </c>
       <c r="C3" s="1">
-        <v>8.7575800000000005E-8</v>
+        <v>9.9677E-8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3242,10 +3301,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>315</v>
+        <v>97</v>
       </c>
       <c r="C4">
-        <v>5.13E-4</v>
+        <v>3.1700000000000001E-4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -3253,10 +3312,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>365</v>
+        <v>93</v>
       </c>
       <c r="C5" s="1">
-        <v>8.9543999999999998E-8</v>
+        <v>1.08871E-7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -3264,10 +3323,43 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>481</v>
+        <v>92</v>
       </c>
       <c r="C6">
-        <v>8.3600000000000005E-4</v>
+        <v>5.5500000000000005E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>92</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4.3100000000000001E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>97</v>
+      </c>
+      <c r="C8">
+        <v>5.6800000000000004E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>97</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1.3136400000000001E-7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>